<commit_message>
Report Adjustment to meet DTF standard
</commit_message>
<xml_diff>
--- a/data/LTD_new.xlsx
+++ b/data/LTD_new.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinaight/Desktop/29mob/ltd_forecasting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6030E9B5-81D5-AF41-893D-0C72782BDA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76BAB66D-B636-A74C-B9BD-5A11A47BEAE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20720" windowHeight="13280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregate data" sheetId="1" r:id="rId1"/>
     <sheet name="LTD and volumes by sector" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -146,6 +160,685 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Data aggregate"/>
+      <sheetName val="Sectoral data"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="2">
+          <cell r="A2">
+            <v>41456</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>41487</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>41518</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>41548</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>41579</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>41609</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>41640</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>41671</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>41699</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>41730</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>41760</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13">
+            <v>41791</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14">
+            <v>41821</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15">
+            <v>41852</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16">
+            <v>41883</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17">
+            <v>41913</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18">
+            <v>41944</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19">
+            <v>41974</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20">
+            <v>42005</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21">
+            <v>42036</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22">
+            <v>42064</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23">
+            <v>42095</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24">
+            <v>42125</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25">
+            <v>42156</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26">
+            <v>42186</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27">
+            <v>42217</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28">
+            <v>42248</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29">
+            <v>42278</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30">
+            <v>42309</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31">
+            <v>42339</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32">
+            <v>42370</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33">
+            <v>42401</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34">
+            <v>42430</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35">
+            <v>42461</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36">
+            <v>42491</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37">
+            <v>42522</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38">
+            <v>42552</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39">
+            <v>42583</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40">
+            <v>42614</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41">
+            <v>42644</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42">
+            <v>42675</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43">
+            <v>42705</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44">
+            <v>42736</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45">
+            <v>42767</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46">
+            <v>42795</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47">
+            <v>42826</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48">
+            <v>42856</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49">
+            <v>42887</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50">
+            <v>42917</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51">
+            <v>42948</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52">
+            <v>42979</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53">
+            <v>43009</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54">
+            <v>43040</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55">
+            <v>43070</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56">
+            <v>43101</v>
+          </cell>
+        </row>
+        <row r="57">
+          <cell r="A57">
+            <v>43132</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="A58">
+            <v>43160</v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59">
+            <v>43191</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60">
+            <v>43221</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61">
+            <v>43252</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62">
+            <v>43282</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63">
+            <v>43313</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64">
+            <v>43344</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65">
+            <v>43374</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66">
+            <v>43405</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67">
+            <v>43435</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68">
+            <v>43466</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69">
+            <v>43497</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70">
+            <v>43525</v>
+          </cell>
+        </row>
+        <row r="71">
+          <cell r="A71">
+            <v>43556</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="A72">
+            <v>43586</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73">
+            <v>43617</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74">
+            <v>43647</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75">
+            <v>43678</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76">
+            <v>43709</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77">
+            <v>43739</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78">
+            <v>43770</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79">
+            <v>43800</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80">
+            <v>43831</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81">
+            <v>43862</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82">
+            <v>43891</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83">
+            <v>43922</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84">
+            <v>43952</v>
+          </cell>
+        </row>
+        <row r="85">
+          <cell r="A85">
+            <v>43983</v>
+          </cell>
+        </row>
+        <row r="86">
+          <cell r="A86">
+            <v>44013</v>
+          </cell>
+        </row>
+        <row r="87">
+          <cell r="A87">
+            <v>44044</v>
+          </cell>
+        </row>
+        <row r="88">
+          <cell r="A88">
+            <v>44075</v>
+          </cell>
+        </row>
+        <row r="89">
+          <cell r="A89">
+            <v>44105</v>
+          </cell>
+        </row>
+        <row r="90">
+          <cell r="A90">
+            <v>44136</v>
+          </cell>
+        </row>
+        <row r="91">
+          <cell r="A91">
+            <v>44166</v>
+          </cell>
+        </row>
+        <row r="92">
+          <cell r="A92">
+            <v>44197</v>
+          </cell>
+        </row>
+        <row r="93">
+          <cell r="A93">
+            <v>44228</v>
+          </cell>
+        </row>
+        <row r="94">
+          <cell r="A94">
+            <v>44256</v>
+          </cell>
+        </row>
+        <row r="95">
+          <cell r="A95">
+            <v>44287</v>
+          </cell>
+        </row>
+        <row r="96">
+          <cell r="A96">
+            <v>44317</v>
+          </cell>
+        </row>
+        <row r="97">
+          <cell r="A97">
+            <v>44348</v>
+          </cell>
+        </row>
+        <row r="98">
+          <cell r="A98">
+            <v>44378</v>
+          </cell>
+        </row>
+        <row r="99">
+          <cell r="A99">
+            <v>44409</v>
+          </cell>
+        </row>
+        <row r="100">
+          <cell r="A100">
+            <v>44440</v>
+          </cell>
+        </row>
+        <row r="101">
+          <cell r="A101">
+            <v>44470</v>
+          </cell>
+        </row>
+        <row r="102">
+          <cell r="A102">
+            <v>44501</v>
+          </cell>
+        </row>
+        <row r="103">
+          <cell r="A103">
+            <v>44531</v>
+          </cell>
+        </row>
+        <row r="104">
+          <cell r="A104">
+            <v>44562</v>
+          </cell>
+        </row>
+        <row r="105">
+          <cell r="A105">
+            <v>44593</v>
+          </cell>
+        </row>
+        <row r="106">
+          <cell r="A106">
+            <v>44621</v>
+          </cell>
+        </row>
+        <row r="107">
+          <cell r="A107">
+            <v>44652</v>
+          </cell>
+        </row>
+        <row r="108">
+          <cell r="A108">
+            <v>44682</v>
+          </cell>
+        </row>
+        <row r="109">
+          <cell r="A109">
+            <v>44713</v>
+          </cell>
+        </row>
+        <row r="110">
+          <cell r="A110">
+            <v>44743</v>
+          </cell>
+        </row>
+        <row r="111">
+          <cell r="A111">
+            <v>44774</v>
+          </cell>
+        </row>
+        <row r="112">
+          <cell r="A112">
+            <v>44805</v>
+          </cell>
+        </row>
+        <row r="113">
+          <cell r="A113">
+            <v>44835</v>
+          </cell>
+        </row>
+        <row r="114">
+          <cell r="A114">
+            <v>44866</v>
+          </cell>
+        </row>
+        <row r="115">
+          <cell r="A115">
+            <v>44896</v>
+          </cell>
+        </row>
+        <row r="116">
+          <cell r="A116">
+            <v>44927</v>
+          </cell>
+        </row>
+        <row r="117">
+          <cell r="A117">
+            <v>44958</v>
+          </cell>
+        </row>
+        <row r="118">
+          <cell r="A118">
+            <v>44986</v>
+          </cell>
+        </row>
+        <row r="119">
+          <cell r="A119">
+            <v>45017</v>
+          </cell>
+        </row>
+        <row r="120">
+          <cell r="A120">
+            <v>45047</v>
+          </cell>
+        </row>
+        <row r="121">
+          <cell r="A121">
+            <v>45078</v>
+          </cell>
+        </row>
+        <row r="122">
+          <cell r="A122">
+            <v>45108</v>
+          </cell>
+        </row>
+        <row r="123">
+          <cell r="A123">
+            <v>45139</v>
+          </cell>
+        </row>
+        <row r="124">
+          <cell r="A124">
+            <v>45170</v>
+          </cell>
+        </row>
+        <row r="125">
+          <cell r="A125">
+            <v>45200</v>
+          </cell>
+        </row>
+        <row r="126">
+          <cell r="A126">
+            <v>45231</v>
+          </cell>
+        </row>
+        <row r="127">
+          <cell r="A127">
+            <v>45261</v>
+          </cell>
+        </row>
+        <row r="128">
+          <cell r="A128">
+            <v>45292</v>
+          </cell>
+        </row>
+        <row r="129">
+          <cell r="A129">
+            <v>45323</v>
+          </cell>
+        </row>
+        <row r="130">
+          <cell r="A130">
+            <v>45352</v>
+          </cell>
+        </row>
+        <row r="131">
+          <cell r="A131">
+            <v>45383</v>
+          </cell>
+        </row>
+        <row r="132">
+          <cell r="A132">
+            <v>45413</v>
+          </cell>
+        </row>
+        <row r="133">
+          <cell r="A133">
+            <v>45444</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A445" workbookViewId="0">
-      <selection activeCell="E194" sqref="E194"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D455" sqref="D455:D457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8918,13 +9611,64 @@
       </c>
     </row>
     <row r="455" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A455" s="1"/>
+      <c r="A455" s="1">
+        <v>45383</v>
+      </c>
+      <c r="B455">
+        <v>700887094.44000006</v>
+      </c>
+      <c r="C455">
+        <v>9590</v>
+      </c>
+      <c r="D455">
+        <v>184.79990000000001</v>
+      </c>
+      <c r="E455">
+        <v>6495.5</v>
+      </c>
+      <c r="F455">
+        <v>8.77</v>
+      </c>
     </row>
     <row r="456" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A456" s="1"/>
+      <c r="A456" s="1">
+        <v>45413</v>
+      </c>
+      <c r="B456">
+        <v>791076300.79999995</v>
+      </c>
+      <c r="C456">
+        <v>10757</v>
+      </c>
+      <c r="D456">
+        <v>184.59639999999999</v>
+      </c>
+      <c r="E456">
+        <v>7270.4</v>
+      </c>
+      <c r="F456">
+        <v>8.77</v>
+      </c>
     </row>
     <row r="457" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A457" s="1"/>
+      <c r="A457" s="1">
+        <v>45444</v>
+      </c>
+      <c r="B457">
+        <v>762042820.17999995</v>
+      </c>
+      <c r="C457">
+        <v>7877</v>
+      </c>
+      <c r="D457">
+        <v>184.25280000000001</v>
+      </c>
+      <c r="E457">
+        <v>8522.2999999999902</v>
+      </c>
+      <c r="F457">
+        <v>8.77</v>
+      </c>
     </row>
     <row r="458" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A458" s="1"/>
@@ -9080,10 +9824,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C84A27EF-AE98-4D0C-A878-1803CF15025B}">
-  <dimension ref="A1:O130"/>
+  <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14790,19 +15534,19 @@
         <v>45108</v>
       </c>
       <c r="B122" s="3">
-        <v>634212641</v>
+        <v>633867201</v>
       </c>
       <c r="C122" s="3">
-        <v>519559271</v>
+        <v>519282448</v>
       </c>
       <c r="D122" s="3">
-        <v>114653370</v>
+        <v>114584753</v>
       </c>
       <c r="E122" s="3">
         <v>46865986</v>
       </c>
       <c r="F122" s="3">
-        <v>39995010</v>
+        <v>39926393</v>
       </c>
       <c r="G122" s="3">
         <v>27792374</v>
@@ -14811,19 +15555,19 @@
         <v>0</v>
       </c>
       <c r="I122" s="3">
-        <v>16502</v>
+        <v>16493</v>
       </c>
       <c r="J122" s="3">
-        <v>15189</v>
+        <v>15182</v>
       </c>
       <c r="K122" s="3">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="L122" s="3">
         <v>467</v>
       </c>
       <c r="M122" s="3">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="N122" s="3">
         <v>416</v>
@@ -14837,10 +15581,10 @@
         <v>45139</v>
       </c>
       <c r="B123" s="3">
-        <v>701096959</v>
+        <v>700837114</v>
       </c>
       <c r="C123" s="3">
-        <v>547066611</v>
+        <v>546806766</v>
       </c>
       <c r="D123" s="3">
         <v>154030348</v>
@@ -14858,10 +15602,10 @@
         <v>0</v>
       </c>
       <c r="I123" s="3">
-        <v>16527</v>
+        <v>16524</v>
       </c>
       <c r="J123" s="3">
-        <v>15460</v>
+        <v>15457</v>
       </c>
       <c r="K123" s="3">
         <v>1067</v>
@@ -14884,19 +15628,19 @@
         <v>45170</v>
       </c>
       <c r="B124" s="3">
-        <v>627913702</v>
+        <v>627491295</v>
       </c>
       <c r="C124" s="3">
-        <v>531472828</v>
+        <v>531357771</v>
       </c>
       <c r="D124" s="3">
-        <v>96440874</v>
+        <v>96133524</v>
       </c>
       <c r="E124" s="3">
         <v>47530096</v>
       </c>
       <c r="F124" s="3">
-        <v>29346054</v>
+        <v>29038704</v>
       </c>
       <c r="G124" s="3">
         <v>19564724</v>
@@ -14905,19 +15649,19 @@
         <v>0</v>
       </c>
       <c r="I124" s="3">
-        <v>16710</v>
+        <v>16702</v>
       </c>
       <c r="J124" s="3">
-        <v>15653</v>
+        <v>15647</v>
       </c>
       <c r="K124" s="3">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="L124" s="3">
         <v>368</v>
       </c>
       <c r="M124" s="3">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="N124" s="3">
         <v>353</v>
@@ -14931,34 +15675,34 @@
         <v>45200</v>
       </c>
       <c r="B125" s="3">
-        <v>692957678</v>
+        <v>692521941</v>
       </c>
       <c r="C125" s="3">
-        <v>560319928</v>
+        <v>560003626</v>
       </c>
       <c r="D125" s="3">
-        <v>132637750</v>
+        <v>132518315</v>
       </c>
       <c r="E125" s="3">
-        <v>71705077</v>
+        <v>71696017</v>
       </c>
       <c r="F125" s="3">
-        <v>36606747</v>
+        <v>36596747</v>
       </c>
       <c r="G125" s="3">
-        <v>24325926</v>
+        <v>24225551</v>
       </c>
       <c r="H125" s="3">
         <v>0</v>
       </c>
       <c r="I125" s="3">
-        <v>17517</v>
+        <v>17514</v>
       </c>
       <c r="J125" s="3">
-        <v>16399</v>
+        <v>16397</v>
       </c>
       <c r="K125" s="3">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="L125" s="3">
         <v>471</v>
@@ -14967,7 +15711,7 @@
         <v>308</v>
       </c>
       <c r="N125" s="3">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="O125" s="3">
         <v>0</v>
@@ -14978,19 +15722,19 @@
         <v>45231</v>
       </c>
       <c r="B126" s="3">
-        <v>701118103</v>
+        <v>700705000</v>
       </c>
       <c r="C126" s="3">
-        <v>597768301</v>
+        <v>597373733</v>
       </c>
       <c r="D126" s="3">
-        <v>103349802</v>
+        <v>103331267</v>
       </c>
       <c r="E126" s="3">
         <v>52115228</v>
       </c>
       <c r="F126" s="3">
-        <v>34553066</v>
+        <v>34534531</v>
       </c>
       <c r="G126" s="3">
         <v>16681508</v>
@@ -14999,10 +15743,10 @@
         <v>0</v>
       </c>
       <c r="I126" s="3">
-        <v>18103</v>
+        <v>18096</v>
       </c>
       <c r="J126" s="3">
-        <v>16890</v>
+        <v>16883</v>
       </c>
       <c r="K126" s="3">
         <v>1213</v>
@@ -15025,40 +15769,40 @@
         <v>45261</v>
       </c>
       <c r="B127" s="3">
-        <v>888372656</v>
+        <v>887968728</v>
       </c>
       <c r="C127" s="3">
-        <v>721439291</v>
+        <v>721341413</v>
       </c>
       <c r="D127" s="3">
-        <v>166933365</v>
+        <v>166627315</v>
       </c>
       <c r="E127" s="3">
-        <v>81683459</v>
+        <v>81378894</v>
       </c>
       <c r="F127" s="3">
-        <v>54495105</v>
+        <v>54534411</v>
       </c>
       <c r="G127" s="3">
-        <v>30754801</v>
+        <v>30714010</v>
       </c>
       <c r="H127" s="3">
         <v>0</v>
       </c>
       <c r="I127" s="3">
-        <v>21452</v>
+        <v>21447</v>
       </c>
       <c r="J127" s="3">
-        <v>19873</v>
+        <v>19869</v>
       </c>
       <c r="K127" s="3">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="L127" s="3">
         <v>653</v>
       </c>
       <c r="M127" s="3">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="N127" s="3">
         <v>438</v>
@@ -15072,40 +15816,40 @@
         <v>45292</v>
       </c>
       <c r="B128" s="3">
-        <v>646502948</v>
+        <v>645750429</v>
       </c>
       <c r="C128" s="3">
-        <v>558163792</v>
+        <v>557524583</v>
       </c>
       <c r="D128" s="3">
-        <v>88339156</v>
+        <v>88225846</v>
       </c>
       <c r="E128" s="3">
-        <v>37342908</v>
+        <v>37343666</v>
       </c>
       <c r="F128" s="3">
-        <v>22146537</v>
+        <v>22021624</v>
       </c>
       <c r="G128" s="3">
-        <v>28849711</v>
+        <v>28860556</v>
       </c>
       <c r="H128" s="3">
         <v>0</v>
       </c>
       <c r="I128" s="3">
-        <v>15181</v>
+        <v>15172</v>
       </c>
       <c r="J128" s="3">
-        <v>14329</v>
+        <v>14321</v>
       </c>
       <c r="K128" s="3">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="L128" s="3">
         <v>284</v>
       </c>
       <c r="M128" s="3">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N128" s="3">
         <v>316</v>
@@ -15119,43 +15863,43 @@
         <v>45323</v>
       </c>
       <c r="B129" s="3">
-        <v>658152214</v>
+        <v>655434556</v>
       </c>
       <c r="C129" s="3">
-        <v>501590450</v>
+        <v>499925985</v>
       </c>
       <c r="D129" s="3">
-        <v>156561764</v>
+        <v>155508571</v>
       </c>
       <c r="E129" s="3">
-        <v>64950082</v>
+        <v>64159783</v>
       </c>
       <c r="F129" s="3">
-        <v>41940078</v>
+        <v>41718027</v>
       </c>
       <c r="G129" s="3">
-        <v>49671604</v>
+        <v>49630761</v>
       </c>
       <c r="H129" s="3">
         <v>0</v>
       </c>
       <c r="I129" s="3">
-        <v>14607</v>
+        <v>14591</v>
       </c>
       <c r="J129" s="3">
-        <v>13539</v>
+        <v>13528</v>
       </c>
       <c r="K129" s="3">
-        <v>1068</v>
+        <v>1063</v>
       </c>
       <c r="L129" s="3">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="M129" s="3">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="N129" s="3">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O129" s="3">
         <v>0</v>
@@ -15166,19 +15910,19 @@
         <v>45352</v>
       </c>
       <c r="B130" s="3">
-        <v>613877846</v>
+        <v>611674565</v>
       </c>
       <c r="C130" s="3">
-        <v>484197139</v>
+        <v>483505506</v>
       </c>
       <c r="D130" s="3">
-        <v>129680707</v>
+        <v>128169059</v>
       </c>
       <c r="E130" s="3">
-        <v>55440560</v>
+        <v>55258915</v>
       </c>
       <c r="F130" s="3">
-        <v>48176814</v>
+        <v>46846811</v>
       </c>
       <c r="G130" s="3">
         <v>26063333</v>
@@ -15187,16 +15931,16 @@
         <v>0</v>
       </c>
       <c r="I130" s="3">
-        <v>15379</v>
+        <v>15366</v>
       </c>
       <c r="J130" s="3">
-        <v>14215</v>
+        <v>14203</v>
       </c>
       <c r="K130" s="3">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="L130" s="3">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M130" s="3">
         <v>356</v>
@@ -15205,6 +15949,147 @@
         <v>372</v>
       </c>
       <c r="O130" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A131" s="4">
+        <v>45383</v>
+      </c>
+      <c r="B131" s="3">
+        <v>653481487</v>
+      </c>
+      <c r="C131" s="3">
+        <v>548257657</v>
+      </c>
+      <c r="D131" s="3">
+        <v>105223830</v>
+      </c>
+      <c r="E131" s="3">
+        <v>51557803</v>
+      </c>
+      <c r="F131" s="3">
+        <v>32672686</v>
+      </c>
+      <c r="G131" s="3">
+        <v>20993341</v>
+      </c>
+      <c r="H131" s="3">
+        <v>0</v>
+      </c>
+      <c r="I131" s="3">
+        <v>17052</v>
+      </c>
+      <c r="J131" s="3">
+        <v>15867</v>
+      </c>
+      <c r="K131" s="3">
+        <v>1185</v>
+      </c>
+      <c r="L131" s="3">
+        <v>429</v>
+      </c>
+      <c r="M131" s="3">
+        <v>347</v>
+      </c>
+      <c r="N131" s="3">
+        <v>409</v>
+      </c>
+      <c r="O131" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A132" s="4">
+        <v>45413</v>
+      </c>
+      <c r="B132" s="3">
+        <v>765007278</v>
+      </c>
+      <c r="C132" s="3">
+        <v>620490152</v>
+      </c>
+      <c r="D132" s="3">
+        <v>144517126</v>
+      </c>
+      <c r="E132" s="3">
+        <v>62710383</v>
+      </c>
+      <c r="F132" s="3">
+        <v>43496781</v>
+      </c>
+      <c r="G132" s="3">
+        <v>38309962</v>
+      </c>
+      <c r="H132" s="3">
+        <v>0</v>
+      </c>
+      <c r="I132" s="3">
+        <v>19322</v>
+      </c>
+      <c r="J132" s="3">
+        <v>18026</v>
+      </c>
+      <c r="K132" s="3">
+        <v>1296</v>
+      </c>
+      <c r="L132" s="3">
+        <v>522</v>
+      </c>
+      <c r="M132" s="3">
+        <v>318</v>
+      </c>
+      <c r="N132" s="3">
+        <v>456</v>
+      </c>
+      <c r="O132" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A133" s="4">
+        <v>45444</v>
+      </c>
+      <c r="B133" s="3">
+        <v>759550343</v>
+      </c>
+      <c r="C133" s="3">
+        <v>600298068</v>
+      </c>
+      <c r="D133" s="3">
+        <v>159252275</v>
+      </c>
+      <c r="E133" s="3">
+        <v>74632249</v>
+      </c>
+      <c r="F133" s="3">
+        <v>64654679</v>
+      </c>
+      <c r="G133" s="3">
+        <v>19965347</v>
+      </c>
+      <c r="H133" s="3">
+        <v>0</v>
+      </c>
+      <c r="I133" s="3">
+        <v>19936</v>
+      </c>
+      <c r="J133" s="3">
+        <v>18367</v>
+      </c>
+      <c r="K133" s="3">
+        <v>1569</v>
+      </c>
+      <c r="L133" s="3">
+        <v>607</v>
+      </c>
+      <c r="M133" s="3">
+        <v>472</v>
+      </c>
+      <c r="N133" s="3">
+        <v>490</v>
+      </c>
+      <c r="O133" s="3">
         <v>0</v>
       </c>
     </row>

</xml_diff>